<commit_message>
Updated Excel files in foldername
</commit_message>
<xml_diff>
--- a/all season cleaned data/allrounderset_ipl.xlsx
+++ b/all season cleaned data/allrounderset_ipl.xlsx
@@ -5,22 +5,34 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/Dataset_Final/cleaned all season/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavanbandaru/Downloads/cricket-squad-selection/all season cleaned data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBCCF7F-1390-6B4E-AF58-F26114B25EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A880A1A8-29D0-DF4E-8AC7-A1B34D209D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="178">
   <si>
     <t>Player</t>
   </si>
@@ -79,15 +91,9 @@
     <t>WG Jacks</t>
   </si>
   <si>
-    <t>100*</t>
-  </si>
-  <si>
     <t>A Kamboj</t>
   </si>
   <si>
-    <t>2*</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -103,15 +109,9 @@
     <t>SZ Mulani</t>
   </si>
   <si>
-    <t>1*</t>
-  </si>
-  <si>
     <t>Naman Dhir</t>
   </si>
   <si>
-    <t>62*</t>
-  </si>
-  <si>
     <t>R Ravindra</t>
   </si>
   <si>
@@ -127,27 +127,18 @@
     <t>Sumit Kumar</t>
   </si>
   <si>
-    <t>9*</t>
-  </si>
-  <si>
     <t>Arshad Khan</t>
   </si>
   <si>
     <t>2023-2024</t>
   </si>
   <si>
-    <t>58*</t>
-  </si>
-  <si>
     <t>Yudhvir Singh</t>
   </si>
   <si>
     <t>K Nitish Kumar Reddy</t>
   </si>
   <si>
-    <t>76*</t>
-  </si>
-  <si>
     <t>Sikandar Raza</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
     <t>Sanvir Singh</t>
   </si>
   <si>
-    <t>8*</t>
-  </si>
-  <si>
     <t>C Green</t>
   </si>
   <si>
@@ -214,24 +202,15 @@
     <t>R Shepherd</t>
   </si>
   <si>
-    <t>39*</t>
-  </si>
-  <si>
     <t>A Badoni</t>
   </si>
   <si>
-    <t>59*</t>
-  </si>
-  <si>
     <t>DJ Mitchell</t>
   </si>
   <si>
     <t>Shashank Singh</t>
   </si>
   <si>
-    <t>68*</t>
-  </si>
-  <si>
     <t>SS Prabhudessai</t>
   </si>
   <si>
@@ -241,9 +220,6 @@
     <t>NT Tilak Varma</t>
   </si>
   <si>
-    <t>84*</t>
-  </si>
-  <si>
     <t>D Pretorius</t>
   </si>
   <si>
@@ -259,9 +235,6 @@
     <t>PN Mankad</t>
   </si>
   <si>
-    <t>64*</t>
-  </si>
-  <si>
     <t>KS Sharma</t>
   </si>
   <si>
@@ -271,9 +244,6 @@
     <t>2022-2022</t>
   </si>
   <si>
-    <t>25*</t>
-  </si>
-  <si>
     <t>RA Bawa</t>
   </si>
   <si>
@@ -286,15 +256,9 @@
     <t>2021-2024</t>
   </si>
   <si>
-    <t>17*</t>
-  </si>
-  <si>
     <t>Lalit Yadav</t>
   </si>
   <si>
-    <t>48*</t>
-  </si>
-  <si>
     <t>VR Iyer</t>
   </si>
   <si>
@@ -328,9 +292,6 @@
     <t>Abdul Samad</t>
   </si>
   <si>
-    <t>37*</t>
-  </si>
-  <si>
     <t>YBK Jaiswal</t>
   </si>
   <si>
@@ -361,15 +322,9 @@
     <t>2019-2024</t>
   </si>
   <si>
-    <t>10*</t>
-  </si>
-  <si>
     <t>SM Curran</t>
   </si>
   <si>
-    <t>63*</t>
-  </si>
-  <si>
     <t>Harpreet Brar</t>
   </si>
   <si>
@@ -382,15 +337,9 @@
     <t>S Dube</t>
   </si>
   <si>
-    <t>95*</t>
-  </si>
-  <si>
     <t>AS Roy</t>
   </si>
   <si>
-    <t>13*</t>
-  </si>
-  <si>
     <t>R Parag</t>
   </si>
   <si>
@@ -412,21 +361,12 @@
     <t>K Gowtham</t>
   </si>
   <si>
-    <t>33*</t>
-  </si>
-  <si>
     <t>Abhishek Sharma</t>
   </si>
   <si>
-    <t>75*</t>
-  </si>
-  <si>
     <t>MK Lomror</t>
   </si>
   <si>
-    <t>54*</t>
-  </si>
-  <si>
     <t>MA Wood</t>
   </si>
   <si>
@@ -436,9 +376,6 @@
     <t>DJ Willey</t>
   </si>
   <si>
-    <t>20*</t>
-  </si>
-  <si>
     <t>TK Curran</t>
   </si>
   <si>
@@ -466,15 +403,9 @@
     <t>2017-2023</t>
   </si>
   <si>
-    <t>107*</t>
-  </si>
-  <si>
     <t>JJ Roy</t>
   </si>
   <si>
-    <t>91*</t>
-  </si>
-  <si>
     <t>KH Pandya</t>
   </si>
   <si>
@@ -484,18 +415,12 @@
     <t>MP Stoinis</t>
   </si>
   <si>
-    <t>124*</t>
-  </si>
-  <si>
     <t>N Rana</t>
   </si>
   <si>
     <t>Swapnil Singh</t>
   </si>
   <si>
-    <t>15*</t>
-  </si>
-  <si>
     <t>SN Thakur</t>
   </si>
   <si>
@@ -529,9 +454,6 @@
     <t>2015-2019</t>
   </si>
   <si>
-    <t>12*</t>
-  </si>
-  <si>
     <t>AR Patel</t>
   </si>
   <si>
@@ -541,9 +463,6 @@
     <t>PJ Cummins</t>
   </si>
   <si>
-    <t>66*</t>
-  </si>
-  <si>
     <t>R Tewatia</t>
   </si>
   <si>
@@ -568,9 +487,6 @@
     <t>2013-2023</t>
   </si>
   <si>
-    <t>47*</t>
-  </si>
-  <si>
     <t>MG Neser</t>
   </si>
   <si>
@@ -583,15 +499,9 @@
     <t>2012-2024</t>
   </si>
   <si>
-    <t>36*</t>
-  </si>
-  <si>
     <t>AD Russell</t>
   </si>
   <si>
-    <t>88*</t>
-  </si>
-  <si>
     <t>GJ Maxwell</t>
   </si>
   <si>
@@ -623,9 +533,6 @@
   </si>
   <si>
     <t>S Dhawan</t>
-  </si>
-  <si>
-    <t>106*</t>
   </si>
   <si>
     <t>Inns</t>
@@ -1031,7 +938,7 @@
   <dimension ref="A1:Z115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1074,28 +981,28 @@
         <v>10</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>207</v>
+        <v>172</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>5</v>
@@ -1116,25 +1023,25 @@
         <v>12</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>209</v>
+        <v>174</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>211</v>
+        <v>176</v>
       </c>
       <c r="Z1" s="2" t="s">
         <v>2</v>
@@ -1242,8 +1149,8 @@
       <c r="G3" s="1">
         <v>230</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
+      <c r="H3" s="1">
+        <v>100</v>
       </c>
       <c r="I3" s="1">
         <v>32.85</v>
@@ -1302,7 +1209,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -1322,11 +1229,11 @@
       <c r="G4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
+      <c r="H4" s="1">
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
@@ -1382,7 +1289,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -1442,13 +1349,13 @@
         <v>0</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V5" s="1">
         <v>12</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X5" s="1">
         <v>0</v>
@@ -1462,7 +1369,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -1510,31 +1417,31 @@
         <v>0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>17</v>
@@ -1542,7 +1449,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>16</v>
@@ -1590,31 +1497,31 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>17</v>
@@ -1622,7 +1529,7 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
@@ -1642,11 +1549,11 @@
       <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
+      <c r="H8" s="1">
+        <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
@@ -1682,13 +1589,13 @@
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V8" s="1">
         <v>11.4</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X8" s="1">
         <v>0</v>
@@ -1702,7 +1609,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
@@ -1722,8 +1629,8 @@
       <c r="G9" s="1">
         <v>140</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>29</v>
+      <c r="H9" s="1">
+        <v>62</v>
       </c>
       <c r="I9" s="1">
         <v>23.33</v>
@@ -1762,13 +1669,13 @@
         <v>0</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V9" s="1">
         <v>11.78</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X9" s="1">
         <v>0</v>
@@ -1782,7 +1689,7 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
@@ -1842,13 +1749,13 @@
         <v>0</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V10" s="1">
         <v>3.5</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X10" s="1">
         <v>0</v>
@@ -1862,7 +1769,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
@@ -1910,31 +1817,31 @@
         <v>2</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z11" s="1" t="s">
         <v>17</v>
@@ -1942,7 +1849,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
@@ -1990,31 +1897,31 @@
         <v>15</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z12" s="1" t="s">
         <v>17</v>
@@ -2022,7 +1929,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -2042,11 +1949,11 @@
       <c r="G13" s="1">
         <v>2</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
+      <c r="H13" s="1">
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1">
         <v>3</v>
@@ -2070,31 +1977,31 @@
         <v>0</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z13" s="1" t="s">
         <v>17</v>
@@ -2102,7 +2009,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>16</v>
@@ -2122,8 +2029,8 @@
       <c r="G14" s="1">
         <v>18</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>35</v>
+      <c r="H14" s="1">
+        <v>9</v>
       </c>
       <c r="I14" s="1">
         <v>9</v>
@@ -2162,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V14" s="1">
         <v>11.4</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X14" s="1">
         <v>0</v>
@@ -2182,10 +2089,10 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -2202,8 +2109,8 @@
       <c r="G15" s="1">
         <v>101</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>38</v>
+      <c r="H15" s="1">
+        <v>58</v>
       </c>
       <c r="I15" s="1">
         <v>25.25</v>
@@ -2262,10 +2169,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -2342,10 +2249,10 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
@@ -2362,8 +2269,8 @@
       <c r="G17" s="1">
         <v>303</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>41</v>
+      <c r="H17" s="1">
+        <v>76</v>
       </c>
       <c r="I17" s="1">
         <v>33.659999999999997</v>
@@ -2422,10 +2329,10 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
         <v>5</v>
@@ -2502,10 +2409,10 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -2582,10 +2489,10 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -2602,8 +2509,8 @@
       <c r="G20" s="1">
         <v>25</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>45</v>
+      <c r="H20" s="1">
+        <v>8</v>
       </c>
       <c r="I20" s="1">
         <v>12.5</v>
@@ -2630,31 +2537,31 @@
         <v>1</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>17</v>
@@ -2662,10 +2569,10 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1">
         <v>10</v>
@@ -2682,8 +2589,8 @@
       <c r="G21" s="1">
         <v>707</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>19</v>
+      <c r="H21" s="1">
+        <v>100</v>
       </c>
       <c r="I21" s="1">
         <v>41.58</v>
@@ -2742,10 +2649,10 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -2822,10 +2729,10 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -2834,40 +2741,40 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q23" s="1">
         <v>6</v>
@@ -2902,10 +2809,10 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -2914,40 +2821,40 @@
         <v>1</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q24" s="1">
         <v>4</v>
@@ -2982,10 +2889,10 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -3002,11 +2909,11 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>27</v>
+      <c r="H25" s="1">
+        <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J25" s="1">
         <v>1</v>
@@ -3030,31 +2937,31 @@
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z25" s="1" t="s">
         <v>17</v>
@@ -3062,10 +2969,10 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -3122,13 +3029,13 @@
         <v>0</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V26" s="1">
         <v>8.42</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -3142,10 +3049,10 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -3190,31 +3097,31 @@
         <v>1</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>17</v>
@@ -3222,10 +3129,10 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1">
         <v>3</v>
@@ -3282,13 +3189,13 @@
         <v>0</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V28" s="1">
         <v>6.25</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X28" s="1">
         <v>0</v>
@@ -3302,10 +3209,10 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -3362,13 +3269,13 @@
         <v>0</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V29" s="1">
         <v>12.33</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X29" s="1">
         <v>0</v>
@@ -3382,10 +3289,10 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -3394,40 +3301,40 @@
         <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q30" s="1">
         <v>6</v>
@@ -3460,10 +3367,10 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -3508,40 +3415,40 @@
         <v>0</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -3598,13 +3505,13 @@
         <v>0</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V32" s="1">
         <v>7</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X32" s="1">
         <v>0</v>
@@ -3616,10 +3523,10 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C33" s="1">
         <v>5</v>
@@ -3696,10 +3603,10 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -3776,10 +3683,10 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C35" s="1">
         <v>9</v>
@@ -3856,10 +3763,10 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C36" s="1">
         <v>0</v>
@@ -3876,8 +3783,8 @@
       <c r="G36" s="1">
         <v>115</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>64</v>
+      <c r="H36" s="1">
+        <v>39</v>
       </c>
       <c r="I36" s="1">
         <v>23</v>
@@ -3936,10 +3843,10 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C37" s="1">
         <v>14</v>
@@ -3956,8 +3863,8 @@
       <c r="G37" s="1">
         <v>634</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>66</v>
+      <c r="H37" s="1">
+        <v>59</v>
       </c>
       <c r="I37" s="1">
         <v>24.38</v>
@@ -4016,10 +3923,10 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C38" s="1">
         <v>11</v>
@@ -4096,10 +4003,10 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C39" s="1">
         <v>10</v>
@@ -4116,8 +4023,8 @@
       <c r="G39" s="1">
         <v>423</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>69</v>
+      <c r="H39" s="1">
+        <v>68</v>
       </c>
       <c r="I39" s="1">
         <v>35.25</v>
@@ -4176,10 +4083,10 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1">
         <v>6</v>
@@ -4224,31 +4131,31 @@
         <v>4</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z40" s="1" t="s">
         <v>17</v>
@@ -4256,10 +4163,10 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
@@ -4304,31 +4211,31 @@
         <v>31</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z41" s="1" t="s">
         <v>17</v>
@@ -4336,10 +4243,10 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C42" s="1">
         <v>23</v>
@@ -4356,8 +4263,8 @@
       <c r="G42" s="1">
         <v>1156</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>73</v>
+      <c r="H42" s="1">
+        <v>84</v>
       </c>
       <c r="I42" s="1">
         <v>39.86</v>
@@ -4396,13 +4303,13 @@
         <v>0</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V42" s="1">
         <v>7.63</v>
       </c>
       <c r="W42" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X42" s="1">
         <v>0</v>
@@ -4416,10 +4323,10 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -4496,10 +4403,10 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C44" s="1">
         <v>5</v>
@@ -4576,10 +4483,10 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C45" s="1">
         <v>9</v>
@@ -4636,13 +4543,13 @@
         <v>0</v>
       </c>
       <c r="U45" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V45" s="1">
         <v>13</v>
       </c>
       <c r="W45" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X45" s="1">
         <v>0</v>
@@ -4656,10 +4563,10 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C46" s="1">
         <v>3</v>
@@ -4676,8 +4583,8 @@
       <c r="G46" s="1">
         <v>97</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>79</v>
+      <c r="H46" s="1">
+        <v>64</v>
       </c>
       <c r="I46" s="1">
         <v>32.33</v>
@@ -4704,31 +4611,31 @@
         <v>2</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z46" s="1" t="s">
         <v>17</v>
@@ -4736,10 +4643,10 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C47" s="1">
         <v>0</v>
@@ -4784,40 +4691,40 @@
         <v>0</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C48" s="1">
         <v>2</v>
@@ -4834,8 +4741,8 @@
       <c r="G48" s="1">
         <v>51</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>83</v>
+      <c r="H48" s="1">
+        <v>25</v>
       </c>
       <c r="I48" s="1">
         <v>17</v>
@@ -4894,10 +4801,10 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C49" s="1">
         <v>0</v>
@@ -4942,31 +4849,31 @@
         <v>0</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z49" s="1" t="s">
         <v>17</v>
@@ -4974,10 +4881,10 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C50" s="1">
         <v>0</v>
@@ -5034,13 +4941,13 @@
         <v>0</v>
       </c>
       <c r="U50" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V50" s="1">
         <v>11.5</v>
       </c>
       <c r="W50" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X50" s="1">
         <v>0</v>
@@ -5054,10 +4961,10 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C51" s="1">
         <v>13</v>
@@ -5074,8 +4981,8 @@
       <c r="G51" s="1">
         <v>66</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>88</v>
+      <c r="H51" s="1">
+        <v>17</v>
       </c>
       <c r="I51" s="1">
         <v>9.42</v>
@@ -5134,10 +5041,10 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C52" s="1">
         <v>16</v>
@@ -5154,8 +5061,8 @@
       <c r="G52" s="1">
         <v>305</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>90</v>
+      <c r="H52" s="1">
+        <v>48</v>
       </c>
       <c r="I52" s="1">
         <v>19.059999999999999</v>
@@ -5214,10 +5121,10 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C53" s="1">
         <v>18</v>
@@ -5294,10 +5201,10 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C54" s="1">
         <v>22</v>
@@ -5342,31 +5249,31 @@
         <v>46</v>
       </c>
       <c r="Q54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y54" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z54" s="1" t="s">
         <v>17</v>
@@ -5374,10 +5281,10 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C55" s="1">
         <v>20</v>
@@ -5434,13 +5341,13 @@
         <v>0</v>
       </c>
       <c r="U55" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V55" s="1">
         <v>7.5</v>
       </c>
       <c r="W55" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X55" s="1">
         <v>0</v>
@@ -5454,10 +5361,10 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C56" s="1">
         <v>2</v>
@@ -5514,13 +5421,13 @@
         <v>0</v>
       </c>
       <c r="U56" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V56" s="1">
         <v>7.33</v>
       </c>
       <c r="W56" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X56" s="1">
         <v>0</v>
@@ -5534,10 +5441,10 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1">
         <v>3</v>
@@ -5612,10 +5519,10 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C58" s="1">
         <v>0</v>
@@ -5624,40 +5531,40 @@
         <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q58" s="1">
         <v>3</v>
@@ -5672,13 +5579,13 @@
         <v>0</v>
       </c>
       <c r="U58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V58" s="1">
         <v>9</v>
       </c>
       <c r="W58" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X58" s="1">
         <v>0</v>
@@ -5692,10 +5599,10 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1">
         <v>21</v>
@@ -5712,8 +5619,8 @@
       <c r="G59" s="1">
         <v>536</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>66</v>
+      <c r="H59" s="1">
+        <v>59</v>
       </c>
       <c r="I59" s="1">
         <v>19.14</v>
@@ -5772,10 +5679,10 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C60" s="1">
         <v>27</v>
@@ -5792,8 +5699,8 @@
       <c r="G60" s="1">
         <v>577</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>102</v>
+      <c r="H60" s="1">
+        <v>37</v>
       </c>
       <c r="I60" s="1">
         <v>19.23</v>
@@ -5852,10 +5759,10 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C61" s="1">
         <v>18</v>
@@ -5912,13 +5819,13 @@
         <v>0</v>
       </c>
       <c r="U61" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V61" s="1">
         <v>36</v>
       </c>
       <c r="W61" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X61" s="1">
         <v>0</v>
@@ -5932,10 +5839,10 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
@@ -6012,10 +5919,10 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C63" s="1">
         <v>10</v>
@@ -6092,10 +5999,10 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C64" s="1">
         <v>4</v>
@@ -6112,8 +6019,8 @@
       <c r="G64" s="1">
         <v>22</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>45</v>
+      <c r="H64" s="1">
+        <v>8</v>
       </c>
       <c r="I64" s="1">
         <v>5.5</v>
@@ -6172,10 +6079,10 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
@@ -6184,40 +6091,40 @@
         <v>1</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q65" s="1">
         <v>2.5</v>
@@ -6232,13 +6139,13 @@
         <v>0</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V65" s="1">
         <v>8.4700000000000006</v>
       </c>
       <c r="W65" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X65" s="1">
         <v>0</v>
@@ -6252,10 +6159,10 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C66" s="1">
         <v>14</v>
@@ -6272,8 +6179,8 @@
       <c r="G66" s="1">
         <v>25</v>
       </c>
-      <c r="H66" s="1" t="s">
-        <v>113</v>
+      <c r="H66" s="1">
+        <v>10</v>
       </c>
       <c r="I66" s="1">
         <v>6.25</v>
@@ -6332,10 +6239,10 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C67" s="1">
         <v>22</v>
@@ -6352,8 +6259,8 @@
       <c r="G67" s="1">
         <v>883</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>115</v>
+      <c r="H67" s="1">
+        <v>63</v>
       </c>
       <c r="I67" s="1">
         <v>25.22</v>
@@ -6412,10 +6319,10 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C68" s="1">
         <v>14</v>
@@ -6492,10 +6399,10 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C69" s="1">
         <v>6</v>
@@ -6572,10 +6479,10 @@
     </row>
     <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C70" s="1">
         <v>18</v>
@@ -6652,10 +6559,10 @@
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C71" s="1">
         <v>19</v>
@@ -6672,8 +6579,8 @@
       <c r="G71" s="1">
         <v>1502</v>
       </c>
-      <c r="H71" s="1" t="s">
-        <v>120</v>
+      <c r="H71" s="1">
+        <v>95</v>
       </c>
       <c r="I71" s="1">
         <v>30.04</v>
@@ -6732,10 +6639,10 @@
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C72" s="1">
         <v>3</v>
@@ -6752,8 +6659,8 @@
       <c r="G72" s="1">
         <v>26</v>
       </c>
-      <c r="H72" s="1" t="s">
-        <v>122</v>
+      <c r="H72" s="1">
+        <v>13</v>
       </c>
       <c r="I72" s="1">
         <v>8.66</v>
@@ -6812,10 +6719,10 @@
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C73" s="1">
         <v>37</v>
@@ -6832,8 +6739,8 @@
       <c r="G73" s="1">
         <v>1173</v>
       </c>
-      <c r="H73" s="1" t="s">
-        <v>73</v>
+      <c r="H73" s="1">
+        <v>84</v>
       </c>
       <c r="I73" s="1">
         <v>24.43</v>
@@ -6892,10 +6799,10 @@
     </row>
     <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C74" s="1">
         <v>5</v>
@@ -6972,10 +6879,10 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C75" s="1">
         <v>1</v>
@@ -6984,40 +6891,40 @@
         <v>1</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q75" s="1">
         <v>2</v>
@@ -7032,13 +6939,13 @@
         <v>0</v>
       </c>
       <c r="U75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V75" s="1">
         <v>13.5</v>
       </c>
       <c r="W75" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X75" s="1">
         <v>0</v>
@@ -7052,10 +6959,10 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C76" s="1">
         <v>22</v>
@@ -7132,10 +7039,10 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C77" s="1">
         <v>17</v>
@@ -7152,8 +7059,8 @@
       <c r="G77" s="1">
         <v>247</v>
       </c>
-      <c r="H77" s="1" t="s">
-        <v>130</v>
+      <c r="H77" s="1">
+        <v>33</v>
       </c>
       <c r="I77" s="1">
         <v>13.72</v>
@@ -7212,10 +7119,10 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C78" s="1">
         <v>17</v>
@@ -7232,8 +7139,8 @@
       <c r="G78" s="1">
         <v>1377</v>
       </c>
-      <c r="H78" s="1" t="s">
-        <v>132</v>
+      <c r="H78" s="1">
+        <v>75</v>
       </c>
       <c r="I78" s="1">
         <v>25.5</v>
@@ -7292,10 +7199,10 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C79" s="1">
         <v>10</v>
@@ -7312,8 +7219,8 @@
       <c r="G79" s="1">
         <v>527</v>
       </c>
-      <c r="H79" s="1" t="s">
-        <v>134</v>
+      <c r="H79" s="1">
+        <v>54</v>
       </c>
       <c r="I79" s="1">
         <v>18.170000000000002</v>
@@ -7372,10 +7279,10 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C80" s="1">
         <v>3</v>
@@ -7392,8 +7299,8 @@
       <c r="G80" s="1">
         <v>12</v>
       </c>
-      <c r="H80" s="1" t="s">
-        <v>113</v>
+      <c r="H80" s="1">
+        <v>10</v>
       </c>
       <c r="I80" s="1">
         <v>6</v>
@@ -7450,10 +7357,10 @@
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C81" s="1">
         <v>4</v>
@@ -7470,8 +7377,8 @@
       <c r="G81" s="1">
         <v>53</v>
       </c>
-      <c r="H81" s="1" t="s">
-        <v>138</v>
+      <c r="H81" s="1">
+        <v>20</v>
       </c>
       <c r="I81" s="1">
         <v>26.5</v>
@@ -7528,10 +7435,10 @@
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="C82" s="1">
         <v>2</v>
@@ -7548,8 +7455,8 @@
       <c r="G82" s="1">
         <v>127</v>
       </c>
-      <c r="H82" s="1" t="s">
-        <v>134</v>
+      <c r="H82" s="1">
+        <v>54</v>
       </c>
       <c r="I82" s="1">
         <v>25.4</v>
@@ -7608,10 +7515,10 @@
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
@@ -7620,40 +7527,40 @@
         <v>1</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q83" s="1">
         <v>3</v>
@@ -7668,13 +7575,13 @@
         <v>0</v>
       </c>
       <c r="U83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V83" s="1">
         <v>11.33</v>
       </c>
       <c r="W83" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X83" s="1">
         <v>0</v>
@@ -7688,10 +7595,10 @@
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="C84" s="1">
         <v>12</v>
@@ -7768,10 +7675,10 @@
     </row>
     <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="C85" s="1">
         <v>18</v>
@@ -7848,10 +7755,10 @@
     </row>
     <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C86" s="1">
         <v>23</v>
@@ -7868,8 +7775,8 @@
       <c r="G86" s="1">
         <v>935</v>
       </c>
-      <c r="H86" s="1" t="s">
-        <v>148</v>
+      <c r="H86" s="1">
+        <v>107</v>
       </c>
       <c r="I86" s="1">
         <v>24.6</v>
@@ -7926,10 +7833,10 @@
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C87" s="1">
         <v>10</v>
@@ -7946,8 +7853,8 @@
       <c r="G87" s="1">
         <v>614</v>
       </c>
-      <c r="H87" s="1" t="s">
-        <v>150</v>
+      <c r="H87" s="1">
+        <v>91</v>
       </c>
       <c r="I87" s="1">
         <v>32.31</v>
@@ -7974,40 +7881,40 @@
         <v>21</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="T87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Z87" s="1"/>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C88" s="1">
         <v>46</v>
@@ -8084,10 +7991,10 @@
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C89" s="1">
         <v>24</v>
@@ -8104,8 +8011,8 @@
       <c r="G89" s="1">
         <v>1866</v>
       </c>
-      <c r="H89" s="1" t="s">
-        <v>154</v>
+      <c r="H89" s="1">
+        <v>124</v>
       </c>
       <c r="I89" s="1">
         <v>28.27</v>
@@ -8164,10 +8071,10 @@
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C90" s="1">
         <v>24</v>
@@ -8244,10 +8151,10 @@
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="C91" s="1">
         <v>3</v>
@@ -8264,8 +8171,8 @@
       <c r="G91" s="1">
         <v>51</v>
       </c>
-      <c r="H91" s="1" t="s">
-        <v>157</v>
+      <c r="H91" s="1">
+        <v>15</v>
       </c>
       <c r="I91" s="1">
         <v>10.199999999999999</v>
@@ -8324,10 +8231,10 @@
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C92" s="1">
         <v>32</v>
@@ -8404,10 +8311,10 @@
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C93" s="1">
         <v>69</v>
@@ -8484,10 +8391,10 @@
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="C94" s="1">
         <v>52</v>
@@ -8564,10 +8471,10 @@
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C95" s="1">
         <v>7</v>
@@ -8644,10 +8551,10 @@
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
       <c r="C96" s="1">
         <v>10</v>
@@ -8704,13 +8611,13 @@
         <v>0</v>
       </c>
       <c r="U96" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V96" s="1">
         <v>18</v>
       </c>
       <c r="W96" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X96" s="1">
         <v>0</v>
@@ -8724,10 +8631,10 @@
     </row>
     <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="C97" s="1">
         <v>1</v>
@@ -8804,10 +8711,10 @@
     </row>
     <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="C98" s="1">
         <v>3</v>
@@ -8824,8 +8731,8 @@
       <c r="G98" s="1">
         <v>24</v>
       </c>
-      <c r="H98" s="1" t="s">
-        <v>169</v>
+      <c r="H98" s="1">
+        <v>12</v>
       </c>
       <c r="I98" s="1">
         <v>8</v>
@@ -8884,10 +8791,10 @@
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C99" s="1">
         <v>72</v>
@@ -8964,10 +8871,10 @@
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C100" s="1">
         <v>15</v>
@@ -8984,8 +8891,8 @@
       <c r="G100" s="1">
         <v>515</v>
       </c>
-      <c r="H100" s="1" t="s">
-        <v>173</v>
+      <c r="H100" s="1">
+        <v>66</v>
       </c>
       <c r="I100" s="1">
         <v>19.8</v>
@@ -9044,10 +8951,10 @@
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C101" s="1">
         <v>38</v>
@@ -9124,10 +9031,10 @@
     </row>
     <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C102" s="1">
         <v>29</v>
@@ -9144,8 +9051,8 @@
       <c r="G102" s="1">
         <v>1115</v>
       </c>
-      <c r="H102" s="1" t="s">
-        <v>115</v>
+      <c r="H102" s="1">
+        <v>63</v>
       </c>
       <c r="I102" s="1">
         <v>25.34</v>
@@ -9204,10 +9111,10 @@
     </row>
     <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="C103" s="1">
         <v>2</v>
@@ -9284,10 +9191,10 @@
     </row>
     <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C104" s="1">
         <v>9</v>
@@ -9304,8 +9211,8 @@
       <c r="G104" s="1">
         <v>210</v>
       </c>
-      <c r="H104" s="1" t="s">
-        <v>83</v>
+      <c r="H104" s="1">
+        <v>25</v>
       </c>
       <c r="I104" s="1">
         <v>19.09</v>
@@ -9364,10 +9271,10 @@
     </row>
     <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="C105" s="1">
         <v>14</v>
@@ -9384,8 +9291,8 @@
       <c r="G105" s="1">
         <v>259</v>
       </c>
-      <c r="H105" s="1" t="s">
-        <v>182</v>
+      <c r="H105" s="1">
+        <v>47</v>
       </c>
       <c r="I105" s="1">
         <v>12.33</v>
@@ -9444,10 +9351,10 @@
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
@@ -9456,40 +9363,40 @@
         <v>1</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q106" s="1">
         <v>4</v>
@@ -9504,13 +9411,13 @@
         <v>0</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="V106" s="1">
         <v>15.5</v>
       </c>
       <c r="W106" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="X106" s="1">
         <v>0</v>
@@ -9524,10 +9431,10 @@
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C107" s="1">
         <v>25</v>
@@ -9544,8 +9451,8 @@
       <c r="G107" s="1">
         <v>249</v>
       </c>
-      <c r="H107" s="1" t="s">
-        <v>187</v>
+      <c r="H107" s="1">
+        <v>36</v>
       </c>
       <c r="I107" s="1">
         <v>9.2200000000000006</v>
@@ -9604,10 +9511,10 @@
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C108" s="1">
         <v>36</v>
@@ -9624,8 +9531,8 @@
       <c r="G108" s="1">
         <v>2484</v>
       </c>
-      <c r="H108" s="1" t="s">
-        <v>189</v>
+      <c r="H108" s="1">
+        <v>88</v>
       </c>
       <c r="I108" s="1">
         <v>29.22</v>
@@ -9684,10 +9591,10 @@
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C109" s="1">
         <v>47</v>
@@ -9764,10 +9671,10 @@
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="C110" s="1">
         <v>14</v>
@@ -9784,8 +9691,8 @@
       <c r="G110" s="1">
         <v>793</v>
       </c>
-      <c r="H110" s="1" t="s">
-        <v>173</v>
+      <c r="H110" s="1">
+        <v>66</v>
       </c>
       <c r="I110" s="1">
         <v>19.82</v>
@@ -9844,10 +9751,10 @@
     </row>
     <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="C111" s="1">
         <v>10</v>
@@ -9924,10 +9831,10 @@
     </row>
     <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="C112" s="1">
         <v>48</v>
@@ -10004,10 +9911,10 @@
     </row>
     <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="C113" s="1">
         <v>103</v>
@@ -10024,8 +9931,8 @@
       <c r="G113" s="1">
         <v>2959</v>
       </c>
-      <c r="H113" s="1" t="s">
-        <v>29</v>
+      <c r="H113" s="1">
+        <v>62</v>
       </c>
       <c r="I113" s="1">
         <v>27.39</v>
@@ -10084,10 +9991,10 @@
     </row>
     <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="C114" s="1">
         <v>23</v>
@@ -10162,10 +10069,10 @@
     </row>
     <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="C115" s="1">
         <v>99</v>
@@ -10182,8 +10089,8 @@
       <c r="G115" s="1">
         <v>6769</v>
       </c>
-      <c r="H115" s="1" t="s">
-        <v>201</v>
+      <c r="H115" s="1">
+        <v>106</v>
       </c>
       <c r="I115" s="1">
         <v>35.25</v>

</xml_diff>